<commit_message>
Updated the Excel Application
Updated the Excel application form
</commit_message>
<xml_diff>
--- a/files/e3application2014form.xlsx
+++ b/files/e3application2014form.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="9880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="E3 Application Form" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'E3 Application Form'!$B$2:$F$43</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -131,6 +131,27 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>June 28</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Orientation</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Deadline:</t>
     </r>
     <r>
@@ -140,7 +161,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Please submit with your resume along with this form before </t>
+      <t xml:space="preserve"> Please submit your resume along with this form before </t>
     </r>
     <r>
       <rPr>
@@ -150,7 +171,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>June 1st</t>
+      <t>June 1, 2014</t>
     </r>
     <r>
       <rPr>
@@ -160,6 +181,27 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> to e3challenge@power-unit.org</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>June 14,15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Group Interviews</t>
     </r>
   </si>
   <si>
@@ -183,57 +225,15 @@
       <t>- Phone Interviews</t>
     </r>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>June 14,15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Group Interviews</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>June 28th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Orientation</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -709,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -949,6 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -974,7 +975,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1142,354 +1143,44 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>55819</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>237286</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>222249</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1477576</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>37820</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1736497</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1171575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 8"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="668140" y="400572"/>
-          <a:ext cx="1421757" cy="1093212"/>
+          <a:off x="3365499" y="0"/>
+          <a:ext cx="3638323" cy="1333500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:blipFill dpi="0" rotWithShape="0">
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-                  <a:grayscl/>
-                </a:blip>
-                <a:srcRect/>
-                <a:stretch>
-                  <a:fillRect/>
-                </a:stretch>
-              </a:blipFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:round/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>876300</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>2679700</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Drop Down 1025" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>1016000</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Check Box 1027" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:ea typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>English</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>1219200</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>2070100</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="Check Box 1028" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Tahoma"/>
-                  <a:ea typeface="Tahoma"/>
-                  <a:cs typeface="Tahoma"/>
-                </a:rPr>
-                <a:t>French</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>2222500</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>101600</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Check Box 1029" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Tahoma"/>
-                  <a:ea typeface="Tahoma"/>
-                  <a:cs typeface="Tahoma"/>
-                </a:rPr>
-                <a:t>Other:</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>88900</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1511300</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1030" name="Drop Down 1031" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1030"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1803,7 +1494,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1845,7 +1536,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1864,49 +1555,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:AA48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="40" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="35" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="21" width="8.83203125" style="1"/>
+    <col min="8" max="21" width="8.85546875" style="1"/>
     <col min="22" max="26" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.83203125" style="1"/>
+    <col min="27" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="101.25" customHeight="1">
-      <c r="B2" s="83" t="s">
+    <row r="2" spans="2:27" ht="112.5" customHeight="1">
+      <c r="B2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="I2" s="77"/>
       <c r="U2" s="3"/>
       <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:27" ht="21">
-      <c r="B3" s="84" t="s">
+    <row r="3" spans="2:27" ht="23.25">
+      <c r="B3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
       <c r="V3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1918,7 +1612,7 @@
       </c>
       <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="2:27" ht="21">
+    <row r="4" spans="2:27" ht="23.25">
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -1929,7 +1623,7 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="6"/>
     </row>
-    <row r="5" spans="2:27" ht="21">
+    <row r="5" spans="2:27" ht="23.25">
       <c r="B5" s="63" t="s">
         <v>31</v>
       </c>
@@ -1944,7 +1638,7 @@
     </row>
     <row r="6" spans="2:27" ht="18.75" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" s="74"/>
       <c r="D6" s="74"/>
@@ -1970,7 +1664,7 @@
     </row>
     <row r="8" spans="2:27" ht="18.75" customHeight="1">
       <c r="B8" s="76" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
@@ -1981,7 +1675,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="2:27" ht="21">
+    <row r="9" spans="2:27" ht="23.25">
       <c r="B9" s="75"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
@@ -1992,9 +1686,9 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="6"/>
     </row>
-    <row r="10" spans="2:27" s="9" customFormat="1" ht="13">
+    <row r="10" spans="2:27" s="9" customFormat="1" ht="15">
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="11"/>
       <c r="E10" s="11"/>
@@ -2014,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="20" customHeight="1">
+    <row r="12" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="16" t="s">
         <v>6</v>
       </c>
@@ -2033,8 +1727,8 @@
       </c>
     </row>
     <row r="13" spans="2:27" ht="7.5" customHeight="1">
-      <c r="B13" s="85"/>
-      <c r="C13" s="86"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="87"/>
       <c r="D13" s="57"/>
       <c r="E13" s="21"/>
       <c r="F13" s="58"/>
@@ -2049,7 +1743,7 @@
       </c>
       <c r="AA13" s="3"/>
     </row>
-    <row r="14" spans="2:27" ht="20" customHeight="1">
+    <row r="14" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
@@ -2071,17 +1765,17 @@
       <c r="AA14" s="3"/>
     </row>
     <row r="15" spans="2:27" ht="12.75" customHeight="1">
-      <c r="B15" s="85"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
       <c r="F15" s="28"/>
       <c r="Z15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="AA15" s="3"/>
     </row>
-    <row r="16" spans="2:27" ht="20" customHeight="1">
+    <row r="16" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
@@ -2098,14 +1792,14 @@
       <c r="AA16" s="3"/>
     </row>
     <row r="17" spans="2:27" ht="12" customHeight="1">
-      <c r="B17" s="85"/>
-      <c r="C17" s="86"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="87"/>
       <c r="D17" s="59"/>
       <c r="E17" s="57"/>
       <c r="F17" s="28"/>
       <c r="AA17" s="3"/>
     </row>
-    <row r="18" spans="2:27" ht="20" customHeight="1">
+    <row r="18" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="23" t="s">
         <v>20</v>
       </c>
@@ -2116,14 +1810,14 @@
       <c r="AA18" s="3"/>
     </row>
     <row r="19" spans="2:27" ht="9" customHeight="1">
-      <c r="B19" s="95"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
       <c r="AA19" s="3"/>
     </row>
-    <row r="20" spans="2:27" ht="20" customHeight="1">
+    <row r="20" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="29" t="s">
         <v>21</v>
       </c>
@@ -2138,20 +1832,20 @@
       <c r="AA20" s="3"/>
     </row>
     <row r="21" spans="2:27" ht="24.75" customHeight="1">
-      <c r="B21" s="85"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="97"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="34"/>
       <c r="F21" s="60"/>
     </row>
     <row r="22" spans="2:27" ht="6" customHeight="1">
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="98"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="35"/>
       <c r="F22" s="36"/>
     </row>
-    <row r="23" spans="2:27" ht="20" customHeight="1">
+    <row r="23" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="23" t="s">
         <v>5</v>
       </c>
@@ -2170,8 +1864,8 @@
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="61"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
     </row>
     <row r="25" spans="2:27" ht="3.75" customHeight="1">
       <c r="B25" s="41"/>
@@ -2180,7 +1874,7 @@
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
-    <row r="26" spans="2:27" ht="20" customHeight="1">
+    <row r="26" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="46" t="s">
         <v>26</v>
       </c>
@@ -2199,18 +1893,18 @@
       <c r="F27" s="51"/>
     </row>
     <row r="28" spans="2:27" s="52" customFormat="1" ht="124.5" customHeight="1">
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
       <c r="V28" s="53"/>
       <c r="W28" s="53"/>
       <c r="X28" s="53"/>
       <c r="Y28" s="53"/>
       <c r="Z28" s="53"/>
     </row>
-    <row r="29" spans="2:27" ht="20" customHeight="1">
+    <row r="29" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B29" s="23" t="s">
         <v>28</v>
       </c>
@@ -2229,13 +1923,13 @@
       <c r="F30" s="55"/>
     </row>
     <row r="31" spans="2:27" ht="124.5" customHeight="1">
-      <c r="B31" s="91"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-    </row>
-    <row r="32" spans="2:27" ht="20" customHeight="1">
+      <c r="B31" s="92"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+    </row>
+    <row r="32" spans="2:27" ht="20.100000000000001" customHeight="1">
       <c r="B32" s="23" t="s">
         <v>29</v>
       </c>
@@ -2254,11 +1948,11 @@
       <c r="F33" s="55"/>
     </row>
     <row r="34" spans="1:18" ht="124.5" customHeight="1" thickBot="1">
-      <c r="B34" s="93"/>
-      <c r="C34" s="94"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
       <c r="O34" s="66"/>
       <c r="P34" s="66"/>
       <c r="Q34" s="66"/>
@@ -2286,11 +1980,11 @@
       <c r="D36" s="54"/>
       <c r="E36" s="54"/>
       <c r="F36" s="70"/>
-      <c r="N36" s="87"/>
-      <c r="O36" s="87"/>
-      <c r="P36" s="87"/>
-      <c r="Q36" s="87"/>
-      <c r="R36" s="87"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="88"/>
+      <c r="P36" s="88"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="88"/>
     </row>
     <row r="37" spans="1:18" ht="16.5" customHeight="1">
       <c r="B37" s="69" t="s">
@@ -2307,61 +2001,61 @@
       <c r="R37" s="64"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="B38" s="77"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="79"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="80"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="B39" s="77"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="79"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="80"/>
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="56"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="79"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="80"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="B41" s="77"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="79"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="80"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="B42" s="77"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="79"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="80"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="B43" s="77"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="79"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="79"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="B44" s="77"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="79"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="80"/>
     </row>
     <row r="45" spans="1:18" ht="31.5" customHeight="1" thickBot="1">
-      <c r="B45" s="80"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="82"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="83"/>
     </row>
     <row r="46" spans="1:18" ht="2.25" customHeight="1">
       <c r="B46" s="65"/>
@@ -2404,132 +2098,10 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.5" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId3" name="Drop Down 1025">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>876300</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>2679700</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId4" name="Check Box 1027">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>1016000</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId5" name="Check Box 1028">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>1219200</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>2070100</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId6" name="Check Box 1029">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>2222500</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>101600</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId7" name="Drop Down 1031">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>88900</xdr:colOff>
-                    <xdr:row>23</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>1511300</xdr:colOff>
-                    <xdr:row>24</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>